<commit_message>
TestCaseBlog changes = add admin and manage page tests
</commit_message>
<xml_diff>
--- a/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/TestCase_Blog.xlsx
+++ b/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/TestCase_Blog.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="570" windowWidth="27495" windowHeight="8895" activeTab="1"/>
+    <workbookView xWindow="150" yWindow="570" windowWidth="20730" windowHeight="8895" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MainBlogPage" sheetId="1" r:id="rId1"/>
     <sheet name="Register Page" sheetId="2" r:id="rId2"/>
+    <sheet name="Manage Page " sheetId="3" r:id="rId3"/>
+    <sheet name="Admin Page " sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Admin Page '!$A$1:$F$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Manage Page '!$A$1:$F$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Register Page'!$A$1:$F$36</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="181">
   <si>
     <t xml:space="preserve">Reference Number </t>
   </si>
@@ -379,13 +384,230 @@
   </si>
   <si>
     <t xml:space="preserve">Hello User ! </t>
+  </si>
+  <si>
+    <t>PasswordChangeWithInvalidSymbols()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"A &lt; and / symbols are not allowed.Please use valid symbols."error message is displayed
+</t>
+  </si>
+  <si>
+    <t>1. &lt;/ input in new password and confirm password fields.
+2. Press ChangePassword button</t>
+  </si>
+  <si>
+    <t>Go to the Manage page- Password Change</t>
+  </si>
+  <si>
+    <t>Change password with invalid data</t>
+  </si>
+  <si>
+    <t>#TC -0009MP -TM</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutData()</t>
+  </si>
+  <si>
+    <t>"The New password field is required."error message is displayed
+"The Current password field is required."error message is displayed
+"The Conform password field is required." error message is displayed - not displayed</t>
+  </si>
+  <si>
+    <t>1. All fields are empty 
+2. Press ChangePassword button</t>
+  </si>
+  <si>
+    <t>Change password without data</t>
+  </si>
+  <si>
+    <t>#TC -0008MP -TM</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutConfirmPassword()</t>
+  </si>
+  <si>
+    <t>"The Confirm password field is required." error message is displayed
+Current message "The password and confirmation password do not match."</t>
+  </si>
+  <si>
+    <t>1. Confirm password field is empty 
+2. Press ChangePassword button</t>
+  </si>
+  <si>
+    <t>Change password without confirm password input</t>
+  </si>
+  <si>
+    <t>#TC -0007MP -TM</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutNewPassword()</t>
+  </si>
+  <si>
+    <t>"The New password field is required."error message is displayed
+"The new password and confirmation password do not match."error message is displayed
+"The Confirm password field is required." error message is displayed - not displayed</t>
+  </si>
+  <si>
+    <t>1. New password field is empty 
+2. Press ChangePassword button</t>
+  </si>
+  <si>
+    <t>Change password without New password input</t>
+  </si>
+  <si>
+    <t>#TC -0006MP -TM</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithWrongCurrentPassword()</t>
+  </si>
+  <si>
+    <t>"Incorrect password." error message is displayed</t>
+  </si>
+  <si>
+    <t>1. Send invalid data in Current password field 
+2. Press ChangePassword button</t>
+  </si>
+  <si>
+    <t>Change password with wrong current password input</t>
+  </si>
+  <si>
+    <t>#TC -0005MP -TM</t>
+  </si>
+  <si>
+    <t>PasswordChangeWithoutCurrentPassword()</t>
+  </si>
+  <si>
+    <t>"The Current password field is required." error message is displayed</t>
+  </si>
+  <si>
+    <t>1. Current password field is empty 
+2. Press ChangePassword button</t>
+  </si>
+  <si>
+    <t>Change password without current password input</t>
+  </si>
+  <si>
+    <t>#TC -0004MP -TM</t>
+  </si>
+  <si>
+    <t>ValidPasswordChangel()</t>
+  </si>
+  <si>
+    <t>"Your password has been changed." message is displayed</t>
+  </si>
+  <si>
+    <t>1. Send valid data in ChangePasswordForm
+2. Press ChangePassword button</t>
+  </si>
+  <si>
+    <t>Enter valid data</t>
+  </si>
+  <si>
+    <t>#TC -0003MP -TM</t>
+  </si>
+  <si>
+    <t>Manage Page - Password change</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NavigatetoPasswordChange()</t>
+  </si>
+  <si>
+    <t>Manage Page - Password change is displayed</t>
+  </si>
+  <si>
+    <t>1. Press ChangeYourPassword button</t>
+  </si>
+  <si>
+    <t>Go to the Manage Page</t>
+  </si>
+  <si>
+    <t>#TC -0002MP -TM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NavigatetoManagePage()</t>
+  </si>
+  <si>
+    <t>Manage Page is displayed</t>
+  </si>
+  <si>
+    <t>1. Press Hello user button</t>
+  </si>
+  <si>
+    <t>Go to the Manage page</t>
+  </si>
+  <si>
+    <t>#TC -0001MP -TM</t>
+  </si>
+  <si>
+    <t>BlogManagePageTests.cs</t>
+  </si>
+  <si>
+    <t>Tatyana Milanova</t>
+  </si>
+  <si>
+    <t>Blog Manage Page</t>
+  </si>
+  <si>
+    <t>Blog Admin Page</t>
+  </si>
+  <si>
+    <t>BlogAdminPageTests.cs</t>
+  </si>
+  <si>
+    <t>#TC -0001AP -TM</t>
+  </si>
+  <si>
+    <t>Go to the Admin user page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logged admin user:Yes - </t>
+  </si>
+  <si>
+    <t>Admin page is displayed</t>
+  </si>
+  <si>
+    <t>NavigateToAdminPage()</t>
+  </si>
+  <si>
+    <t>#TC -0002AP -TM</t>
+  </si>
+  <si>
+    <t>Go to the Admin page - Users List</t>
+  </si>
+  <si>
+    <t>Logged admin  user:Yes</t>
+  </si>
+  <si>
+    <t>Users list is displayed</t>
+  </si>
+  <si>
+    <t>NavigateToAdminPageUserManage()</t>
+  </si>
+  <si>
+    <t>Admin Page - Users</t>
+  </si>
+  <si>
+    <t>#TC -0003AP -TM</t>
+  </si>
+  <si>
+    <t>Edit user info by admin</t>
+  </si>
+  <si>
+    <t>Logged admin user:Yes</t>
+  </si>
+  <si>
+    <t>"Change user data is successful" message is displayed.</t>
+  </si>
+  <si>
+    <t>да допълня аналогични на регистрацията тестове плюс изтриване на потребител и на админ. Да може ли да се изтрива админ?!?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -444,6 +666,13 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -512,7 +741,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -598,11 +827,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -740,6 +989,63 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,7 +1136,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -865,7 +1170,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1041,14 +1345,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="30.140625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -1059,7 +1363,7 @@
     <col min="7" max="7" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="12.75">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1375,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="12.75">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1083,7 +1387,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="12.75">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1093,7 +1397,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="12.75">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1105,7 +1409,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="12.75">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -1117,7 +1421,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1129,7 +1433,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="12.75">
       <c r="A7" s="13" t="s">
         <v>66</v>
       </c>
@@ -1141,7 +1445,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="12.75">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1151,7 +1455,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="12.75">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1159,7 +1463,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="12.75">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1188,7 +1492,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="28.5">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -1231,7 +1535,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="35.25" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>75</v>
       </c>
@@ -1272,7 +1576,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="17.25" customHeight="1">
       <c r="A13" s="35" t="s">
         <v>77</v>
       </c>
@@ -1303,7 +1607,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="35.25" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>76</v>
       </c>
@@ -1346,7 +1650,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="25.5">
       <c r="A15" s="32" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1691,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="14.25" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +1732,7 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="38.25">
       <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
@@ -1469,7 +1773,7 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="12.75">
       <c r="A18" s="6" t="s">
         <v>87</v>
       </c>
@@ -1500,7 +1804,7 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="25.5">
       <c r="A19" s="11" t="s">
         <v>52</v>
       </c>
@@ -1541,7 +1845,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="25.5">
       <c r="A20" s="37" t="s">
         <v>53</v>
       </c>
@@ -1582,7 +1886,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="25.5" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>54</v>
       </c>
@@ -1623,7 +1927,7 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="12.75">
       <c r="A22" s="41"/>
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
@@ -1652,7 +1956,7 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="12.75">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="3"/>
@@ -1660,7 +1964,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="12.75">
       <c r="A24" s="16" t="s">
         <v>16</v>
       </c>
@@ -1670,7 +1974,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="12.75">
       <c r="A25" s="19" t="s">
         <v>10</v>
       </c>
@@ -1682,7 +1986,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="12.75">
       <c r="A26" s="19" t="s">
         <v>17</v>
       </c>
@@ -1694,7 +1998,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="12.75">
       <c r="A27" s="19" t="s">
         <v>11</v>
       </c>
@@ -1706,7 +2010,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="12.75">
       <c r="A28" s="19" t="s">
         <v>12</v>
       </c>
@@ -1718,7 +2022,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="12.75">
       <c r="A29" s="19" t="s">
         <v>13</v>
       </c>
@@ -1730,7 +2034,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="12.75">
       <c r="A30" s="19" t="s">
         <v>18</v>
       </c>
@@ -1742,7 +2046,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="12.75">
       <c r="A31" s="19" t="s">
         <v>19</v>
       </c>
@@ -1754,7 +2058,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -1769,14 +2073,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -1787,7 +2091,7 @@
     <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="12.75">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1799,7 +2103,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="12.75">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1811,7 +2115,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="12.75">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1821,7 +2125,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="12.75">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1833,7 +2137,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="12.75">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -1845,7 +2149,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1857,7 +2161,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="12.75">
       <c r="A7" s="13" t="s">
         <v>66</v>
       </c>
@@ -1869,7 +2173,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="12.75">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1879,7 +2183,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="12.75">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1887,7 +2191,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="12.75">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1916,7 +2220,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="28.5">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -1959,7 +2263,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="35.25" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>22</v>
       </c>
@@ -2000,7 +2304,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="12.75">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2031,7 +2335,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="38.25">
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
@@ -2074,7 +2378,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="25.5">
       <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
@@ -2117,7 +2421,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="38.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -2160,7 +2464,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="12.75">
       <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
@@ -2191,7 +2495,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="34.5" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>39</v>
       </c>
@@ -2234,7 +2538,7 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="25.5" customHeight="1">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -2263,7 +2567,7 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="12.75">
       <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
@@ -2294,7 +2598,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="34.5" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>53</v>
       </c>
@@ -2337,7 +2641,7 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="51">
       <c r="A22" s="11" t="s">
         <v>54</v>
       </c>
@@ -2380,7 +2684,7 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="38.25">
       <c r="A23" s="11" t="s">
         <v>69</v>
       </c>
@@ -2423,7 +2727,7 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="12.75">
       <c r="A24" s="6" t="s">
         <v>108</v>
       </c>
@@ -2454,7 +2758,7 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="34.5" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>109</v>
       </c>
@@ -2495,7 +2799,7 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="26.25" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2524,7 +2828,7 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="61.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="3"/>
@@ -2532,7 +2836,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="12.75">
       <c r="A28" s="16" t="s">
         <v>16</v>
       </c>
@@ -2542,7 +2846,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="12.75">
       <c r="A29" s="19" t="s">
         <v>10</v>
       </c>
@@ -2554,7 +2858,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="12.75">
       <c r="A30" s="19" t="s">
         <v>17</v>
       </c>
@@ -2566,7 +2870,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="12.75">
       <c r="A31" s="19" t="s">
         <v>11</v>
       </c>
@@ -2578,7 +2882,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="12.75">
       <c r="A32" s="19" t="s">
         <v>12</v>
       </c>
@@ -2590,7 +2894,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="12.75">
       <c r="A33" s="19" t="s">
         <v>13</v>
       </c>
@@ -2602,7 +2906,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="12.75">
       <c r="A34" s="19" t="s">
         <v>18</v>
       </c>
@@ -2614,7 +2918,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="12.75">
       <c r="A35" s="19" t="s">
         <v>19</v>
       </c>
@@ -2626,7 +2930,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -2634,7 +2938,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2642,7 +2946,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2650,7 +2954,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2658,7 +2962,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2666,7 +2970,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2674,7 +2978,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2682,7 +2986,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2690,7 +2994,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2698,7 +3002,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2710,4 +3014,1404 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA42"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" style="54" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="54" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="54" customWidth="1"/>
+    <col min="4" max="4" width="9" style="54" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="54" customWidth="1"/>
+    <col min="6" max="6" width="67" style="54" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="14.42578125" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="12.75">
+      <c r="A1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+    </row>
+    <row r="2" spans="1:27" ht="12.75">
+      <c r="A2" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+    </row>
+    <row r="3" spans="1:27" ht="12.75">
+      <c r="A3" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="68"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+    </row>
+    <row r="4" spans="1:27" ht="12.75">
+      <c r="A4" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+    </row>
+    <row r="5" spans="1:27" ht="12.75">
+      <c r="A5" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+    </row>
+    <row r="6" spans="1:27" ht="12.75">
+      <c r="A6" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+    </row>
+    <row r="7" spans="1:27" ht="12.75">
+      <c r="A7" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+    </row>
+    <row r="8" spans="1:27" ht="12.75">
+      <c r="A8" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="68"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+    </row>
+    <row r="9" spans="1:27" ht="12.75">
+      <c r="A9" s="67"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+    </row>
+    <row r="10" spans="1:27" ht="12.75">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="61"/>
+      <c r="S10" s="61"/>
+      <c r="T10" s="61"/>
+      <c r="U10" s="61"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="61"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="61"/>
+      <c r="Z10" s="61"/>
+      <c r="AA10" s="61"/>
+    </row>
+    <row r="11" spans="1:27" ht="28.5">
+      <c r="A11" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="61"/>
+      <c r="U11" s="61"/>
+      <c r="V11" s="61"/>
+      <c r="W11" s="61"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="61"/>
+      <c r="Z11" s="61"/>
+      <c r="AA11" s="61"/>
+    </row>
+    <row r="12" spans="1:27" ht="35.25" customHeight="1">
+      <c r="A12" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="61"/>
+      <c r="U12" s="61"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="61"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="61"/>
+      <c r="Z12" s="61"/>
+      <c r="AA12" s="61"/>
+    </row>
+    <row r="13" spans="1:27" ht="35.25" customHeight="1">
+      <c r="A13" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="61"/>
+      <c r="T13" s="61"/>
+      <c r="U13" s="61"/>
+      <c r="V13" s="61"/>
+      <c r="W13" s="61"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="61"/>
+      <c r="AA13" s="61"/>
+    </row>
+    <row r="14" spans="1:27" ht="35.25" customHeight="1">
+      <c r="A14" s="63"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="61"/>
+      <c r="T14" s="61"/>
+      <c r="U14" s="61"/>
+      <c r="V14" s="61"/>
+      <c r="W14" s="61"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="61"/>
+      <c r="Z14" s="61"/>
+      <c r="AA14" s="61"/>
+    </row>
+    <row r="15" spans="1:27" ht="25.5" customHeight="1">
+      <c r="A15" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="61"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="61"/>
+      <c r="U15" s="61"/>
+      <c r="V15" s="61"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="61"/>
+      <c r="Y15" s="61"/>
+      <c r="Z15" s="61"/>
+      <c r="AA15" s="61"/>
+    </row>
+    <row r="16" spans="1:27" ht="51">
+      <c r="A16" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="9">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="61"/>
+      <c r="R16" s="61"/>
+      <c r="S16" s="61"/>
+      <c r="T16" s="61"/>
+      <c r="U16" s="61"/>
+      <c r="V16" s="61"/>
+      <c r="W16" s="61"/>
+      <c r="X16" s="61"/>
+      <c r="Y16" s="61"/>
+      <c r="Z16" s="61"/>
+      <c r="AA16" s="61"/>
+    </row>
+    <row r="17" spans="1:27" ht="51">
+      <c r="A17" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="61"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="61"/>
+      <c r="S17" s="61"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="61"/>
+      <c r="V17" s="61"/>
+      <c r="W17" s="61"/>
+      <c r="X17" s="61"/>
+      <c r="Y17" s="61"/>
+      <c r="Z17" s="61"/>
+      <c r="AA17" s="61"/>
+    </row>
+    <row r="18" spans="1:27" ht="51">
+      <c r="A18" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="53" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="61"/>
+      <c r="AA18" s="61"/>
+    </row>
+    <row r="19" spans="1:27" ht="63.75">
+      <c r="A19" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="61"/>
+      <c r="S19" s="61"/>
+      <c r="T19" s="61"/>
+      <c r="U19" s="61"/>
+      <c r="V19" s="61"/>
+      <c r="W19" s="61"/>
+      <c r="X19" s="61"/>
+      <c r="Y19" s="61"/>
+      <c r="Z19" s="61"/>
+      <c r="AA19" s="61"/>
+    </row>
+    <row r="20" spans="1:27" ht="51">
+      <c r="A20" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="61"/>
+      <c r="U20" s="61"/>
+      <c r="V20" s="61"/>
+      <c r="W20" s="61"/>
+      <c r="X20" s="61"/>
+      <c r="Y20" s="61"/>
+      <c r="Z20" s="61"/>
+      <c r="AA20" s="61"/>
+    </row>
+    <row r="21" spans="1:27" ht="51">
+      <c r="A21" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="12">
+        <v>2</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="62"/>
+      <c r="T21" s="62"/>
+      <c r="U21" s="62"/>
+      <c r="V21" s="62"/>
+      <c r="W21" s="62"/>
+      <c r="X21" s="62"/>
+      <c r="Y21" s="62"/>
+      <c r="Z21" s="62"/>
+      <c r="AA21" s="62"/>
+    </row>
+    <row r="22" spans="1:27" ht="51">
+      <c r="A22" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="12">
+        <v>2</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="62"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="62"/>
+      <c r="T22" s="62"/>
+      <c r="U22" s="62"/>
+      <c r="V22" s="62"/>
+      <c r="W22" s="62"/>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="62"/>
+      <c r="Z22" s="62"/>
+      <c r="AA22" s="62"/>
+    </row>
+    <row r="23" spans="1:27" ht="26.25" customHeight="1">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="61"/>
+      <c r="R23" s="61"/>
+      <c r="S23" s="61"/>
+      <c r="T23" s="61"/>
+      <c r="U23" s="61"/>
+      <c r="V23" s="61"/>
+      <c r="W23" s="61"/>
+      <c r="X23" s="61"/>
+      <c r="Y23" s="61"/>
+      <c r="Z23" s="61"/>
+      <c r="AA23" s="61"/>
+    </row>
+    <row r="24" spans="1:27" ht="61.5" customHeight="1">
+      <c r="A24" s="60"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+    </row>
+    <row r="25" spans="1:27" ht="12.75">
+      <c r="A25" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="58"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+    </row>
+    <row r="26" spans="1:27" ht="25.5">
+      <c r="A26" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+    </row>
+    <row r="27" spans="1:27" ht="12.75">
+      <c r="A27" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+    </row>
+    <row r="28" spans="1:27" ht="12.75">
+      <c r="A28" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="57"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+    </row>
+    <row r="29" spans="1:27" ht="12.75">
+      <c r="A29" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="57"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+    </row>
+    <row r="30" spans="1:27" ht="12.75">
+      <c r="A30" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="57"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+    </row>
+    <row r="31" spans="1:27" ht="12.75">
+      <c r="A31" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="57"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+    </row>
+    <row r="32" spans="1:27" ht="12.75">
+      <c r="A32" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A33" s="56"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A34" s="55"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A35" s="55"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A36" s="55"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A37" s="55"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A38" s="55"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A39" s="55"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A40" s="55"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A41" s="55"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A42" s="55"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:G15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="67" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="12.75">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:27" ht="12.75">
+      <c r="A2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:27" ht="12.75">
+      <c r="A3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:27" ht="12.75">
+      <c r="A4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" ht="12.75">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" ht="12.75">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:27" ht="12.75">
+      <c r="A7" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="12.75">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" ht="12.75">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:27" ht="12.75">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" ht="28.5">
+      <c r="A11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" ht="35.25" customHeight="1">
+      <c r="A12" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" ht="35.25" customHeight="1">
+      <c r="A13" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" ht="12.75">
+      <c r="A14" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" ht="26.25" customHeight="1">
+      <c r="A15" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="G15" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" ht="61.5" customHeight="1">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="12.75">
+      <c r="A17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="12.75">
+      <c r="A18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="12.75">
+      <c r="A19" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="12.75">
+      <c r="A20" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="12.75">
+      <c r="A21" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.75">
+      <c r="A22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="12.75">
+      <c r="A23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" ht="12.75">
+      <c r="A24" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Log in Page Test Cases
Adding Log in Page Test Cases
</commit_message>
<xml_diff>
--- a/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/TestCase_Blog.xlsx
+++ b/BartlettAreTheQAs/BartlettAreTheQAs/ExcelFilesData/TestCase_Blog.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="150" yWindow="570" windowWidth="20730" windowHeight="8895" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MainBlogPage" sheetId="1" r:id="rId1"/>
     <sheet name="Register Page" sheetId="2" r:id="rId2"/>
     <sheet name="Manage Page " sheetId="3" r:id="rId3"/>
     <sheet name="Admin Page " sheetId="5" r:id="rId4"/>
+    <sheet name="Login Page" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Admin Page '!$A$1:$F$32</definedName>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="268">
   <si>
     <t xml:space="preserve">Reference Number </t>
   </si>
@@ -740,13 +746,155 @@
   </si>
   <si>
     <t>DeleteUser()</t>
+  </si>
+  <si>
+    <t>Blog Login Page</t>
+  </si>
+  <si>
+    <t>Neli Koynarska(nellysiko)</t>
+  </si>
+  <si>
+    <t>#TC -0001LP -NK</t>
+  </si>
+  <si>
+    <t>#TC -0003LP -NK</t>
+  </si>
+  <si>
+    <t>#TC -0002LP -NK</t>
+  </si>
+  <si>
+    <t>#TC -0004LP -NK</t>
+  </si>
+  <si>
+    <t>#TC -0005LP -NK</t>
+  </si>
+  <si>
+    <t>#TC -0006LP -NK</t>
+  </si>
+  <si>
+    <t>#TC -0007LP -NK</t>
+  </si>
+  <si>
+    <t>#TC -0008LP -NK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log in Remember me </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to Log in Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log in Successfully </t>
+  </si>
+  <si>
+    <t>Log in With Wrong Email</t>
+  </si>
+  <si>
+    <t>Log in With Wrong Password</t>
+  </si>
+  <si>
+    <t>Log in Without Data</t>
+  </si>
+  <si>
+    <t>Log in Without Email</t>
+  </si>
+  <si>
+    <t>Log in Without Pass</t>
+  </si>
+  <si>
+    <t>Log in Page -Successfully</t>
+  </si>
+  <si>
+    <t>Log in Page -Wrong Data</t>
+  </si>
+  <si>
+    <t>Log in Page -Without Data</t>
+  </si>
+  <si>
+    <t>Log in Page - Remember me</t>
+  </si>
+  <si>
+    <t>Log in Page is displayed</t>
+  </si>
+  <si>
+    <t>NavigateToLogInPage()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send Valid Email string 
+2. Send Valid Password          3. Press Log in Button </t>
+  </si>
+  <si>
+    <t>"Log off" button is displayed</t>
+  </si>
+  <si>
+    <t>LogInSuccessfully()</t>
+  </si>
+  <si>
+    <t>Go to Log in Page</t>
+  </si>
+  <si>
+    <t>LogInWithWrongEmail()</t>
+  </si>
+  <si>
+    <t>LogInWithWrongPassword()</t>
+  </si>
+  <si>
+    <t>LogInWithoutData()</t>
+  </si>
+  <si>
+    <t>LogInWithoutEmail()</t>
+  </si>
+  <si>
+    <t>LogInWithoutPass()</t>
+  </si>
+  <si>
+    <t>LogInRememberMe()</t>
+  </si>
+  <si>
+    <t>"Invalid login attempt."</t>
+  </si>
+  <si>
+    <t>"The email field is not a valid e-mail address."</t>
+  </si>
+  <si>
+    <t>1. Press "Log in" button</t>
+  </si>
+  <si>
+    <t>"The email field is requited."                "The Password field is required."</t>
+  </si>
+  <si>
+    <t>1. Send Valid Password          2. Press Log in Button</t>
+  </si>
+  <si>
+    <t>"The email field is requared."</t>
+  </si>
+  <si>
+    <t>1. Send Valid Email               2. Press Log in Button</t>
+  </si>
+  <si>
+    <t>"The Password field is required."</t>
+  </si>
+  <si>
+    <t>"Lof off" button is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send Invalid Email string 
+2. Send Valid Password          3. Press Log in Button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send Valid Email string 
+2. Send Invalid Password          3. Press Log in Button </t>
+  </si>
+  <si>
+    <t>1. Send Valid Email string 
+2. Send Valid Password          3. Press Check box              4. Press Log in Button  button"Remember me"          5. Go to www.google.com     6. Go to Main Blog Page (locallhost:60634/Article/List)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1010,7 +1158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1194,37 +1342,43 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,6 +1388,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1282,7 +1439,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1314,9 +1471,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1348,6 +1506,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1523,14 +1682,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.140625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -1541,7 +1700,7 @@
     <col min="7" max="7" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75">
+    <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1553,7 +1712,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75">
+    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1565,7 +1724,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1575,7 +1734,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1587,7 +1746,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -1599,7 +1758,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75">
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1611,7 +1770,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="12.75">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>64</v>
       </c>
@@ -1623,7 +1782,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1633,7 +1792,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="12.75">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1641,7 +1800,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="12.75">
+    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1670,7 +1829,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="28.5">
+    <row r="11" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -1713,7 +1872,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="35.25" customHeight="1">
+    <row r="12" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>73</v>
       </c>
@@ -1754,7 +1913,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="17.25" customHeight="1">
+    <row r="13" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>75</v>
       </c>
@@ -1785,7 +1944,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="35.25" customHeight="1">
+    <row r="14" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>74</v>
       </c>
@@ -1828,7 +1987,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="25.5">
+    <row r="15" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>26</v>
       </c>
@@ -1871,7 +2030,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1">
+    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1900,7 +2059,7 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="1:27" ht="12.75">
+    <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1929,7 +2088,7 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" ht="12.75">
+    <row r="18" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>82</v>
       </c>
@@ -1960,7 +2119,7 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="25.5">
+    <row r="19" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>174</v>
       </c>
@@ -2001,7 +2160,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="25.5">
+    <row r="20" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
         <v>175</v>
       </c>
@@ -2042,7 +2201,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="25.5" customHeight="1">
+    <row r="21" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>176</v>
       </c>
@@ -2083,7 +2242,7 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="55.5" customHeight="1">
+    <row r="22" spans="1:27" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="66" t="s">
         <v>177</v>
       </c>
@@ -2126,7 +2285,7 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="71.25" customHeight="1">
+    <row r="23" spans="1:27" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="66" t="s">
         <v>177</v>
       </c>
@@ -2149,7 +2308,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="12.75">
+    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="3"/>
@@ -2157,7 +2316,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:27" ht="12.75">
+    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>16</v>
       </c>
@@ -2167,7 +2326,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:27" ht="12.75">
+    <row r="26" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>10</v>
       </c>
@@ -2179,7 +2338,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:27" ht="12.75">
+    <row r="27" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>17</v>
       </c>
@@ -2191,7 +2350,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:27" ht="12.75">
+    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>11</v>
       </c>
@@ -2203,7 +2362,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="12.75">
+    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>12</v>
       </c>
@@ -2215,7 +2374,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:27" ht="12.75">
+    <row r="30" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>13</v>
       </c>
@@ -2227,7 +2386,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:27" ht="12.75">
+    <row r="31" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>18</v>
       </c>
@@ -2239,7 +2398,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" customHeight="1">
+    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>19</v>
       </c>
@@ -2251,7 +2410,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -2266,14 +2425,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -2284,7 +2443,7 @@
     <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75">
+    <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2296,7 +2455,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75">
+    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -2308,7 +2467,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -2318,7 +2477,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -2330,7 +2489,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -2342,7 +2501,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75">
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -2354,7 +2513,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="12.75">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>64</v>
       </c>
@@ -2366,7 +2525,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -2376,7 +2535,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="12.75">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2384,7 +2543,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="12.75">
+    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2413,7 +2572,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="28.5">
+    <row r="11" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -2456,7 +2615,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="35.25" customHeight="1">
+    <row r="12" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>22</v>
       </c>
@@ -2497,7 +2656,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="12.75">
+    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2528,7 +2687,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="38.25">
+    <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
@@ -2571,7 +2730,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="25.5">
+    <row r="15" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
@@ -2614,7 +2773,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="38.25">
+    <row r="16" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -2657,7 +2816,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="12.75">
+    <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
@@ -2688,7 +2847,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="34.5" customHeight="1">
+    <row r="18" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>39</v>
       </c>
@@ -2731,7 +2890,7 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="25.5" customHeight="1">
+    <row r="19" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -2760,7 +2919,7 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="1:27" ht="12.75">
+    <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
@@ -2791,7 +2950,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="34.5" customHeight="1">
+    <row r="21" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
@@ -2834,7 +2993,7 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="38.25">
+    <row r="22" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>52</v>
       </c>
@@ -2877,7 +3036,7 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" ht="38.25">
+    <row r="23" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>67</v>
       </c>
@@ -2920,7 +3079,7 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="12.75">
+    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -2951,7 +3110,7 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="34.5" customHeight="1">
+    <row r="25" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>102</v>
       </c>
@@ -2992,7 +3151,7 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" ht="26.25" customHeight="1">
+    <row r="26" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3021,7 +3180,7 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="61.5" customHeight="1">
+    <row r="27" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="3"/>
@@ -3029,7 +3188,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:27" ht="12.75">
+    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>16</v>
       </c>
@@ -3039,7 +3198,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="12.75">
+    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>10</v>
       </c>
@@ -3051,7 +3210,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:27" ht="12.75">
+    <row r="30" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>17</v>
       </c>
@@ -3063,7 +3222,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:27" ht="12.75">
+    <row r="31" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>11</v>
       </c>
@@ -3075,7 +3234,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:27" ht="12.75">
+    <row r="32" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>12</v>
       </c>
@@ -3087,7 +3246,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="12.75">
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>13</v>
       </c>
@@ -3099,7 +3258,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="12.75">
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>18</v>
       </c>
@@ -3111,7 +3270,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="12.75">
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>19</v>
       </c>
@@ -3123,7 +3282,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -3131,7 +3290,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -3139,7 +3298,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -3147,7 +3306,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -3155,7 +3314,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -3163,7 +3322,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -3171,7 +3330,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -3179,7 +3338,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3187,7 +3346,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -3195,7 +3354,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -3210,14 +3369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.140625" style="49" customWidth="1"/>
     <col min="2" max="2" width="45.140625" style="49" customWidth="1"/>
@@ -3229,7 +3388,7 @@
     <col min="8" max="16384" width="14.42578125" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75">
+    <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
@@ -3241,7 +3400,7 @@
       <c r="E1" s="50"/>
       <c r="F1" s="50"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75">
+    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="63" t="s">
         <v>2</v>
       </c>
@@ -3253,7 +3412,7 @@
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
@@ -3263,7 +3422,7 @@
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="63" t="s">
         <v>4</v>
       </c>
@@ -3275,7 +3434,7 @@
       <c r="E4" s="50"/>
       <c r="F4" s="50"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="63" t="s">
         <v>5</v>
       </c>
@@ -3287,7 +3446,7 @@
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75">
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="63" t="s">
         <v>7</v>
       </c>
@@ -3299,7 +3458,7 @@
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
     </row>
-    <row r="7" spans="1:27" ht="12.75">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="63" t="s">
         <v>64</v>
       </c>
@@ -3311,7 +3470,7 @@
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="63" t="s">
         <v>9</v>
       </c>
@@ -3321,7 +3480,7 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
     </row>
-    <row r="9" spans="1:27" ht="12.75">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="62"/>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -3329,7 +3488,7 @@
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
     </row>
-    <row r="10" spans="1:27" ht="12.75">
+    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -3358,7 +3517,7 @@
       <c r="Z10" s="56"/>
       <c r="AA10" s="56"/>
     </row>
-    <row r="11" spans="1:27" ht="28.5">
+    <row r="11" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="61" t="s">
         <v>10</v>
       </c>
@@ -3401,7 +3560,7 @@
       <c r="Z11" s="56"/>
       <c r="AA11" s="56"/>
     </row>
-    <row r="12" spans="1:27" ht="35.25" customHeight="1">
+    <row r="12" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>152</v>
       </c>
@@ -3444,7 +3603,7 @@
       <c r="Z12" s="56"/>
       <c r="AA12" s="56"/>
     </row>
-    <row r="13" spans="1:27" ht="35.25" customHeight="1">
+    <row r="13" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
         <v>147</v>
       </c>
@@ -3487,7 +3646,7 @@
       <c r="Z13" s="56"/>
       <c r="AA13" s="56"/>
     </row>
-    <row r="14" spans="1:27" ht="35.25" customHeight="1">
+    <row r="14" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="58"/>
       <c r="B14" s="58"/>
       <c r="C14" s="59"/>
@@ -3516,16 +3675,16 @@
       <c r="Z14" s="56"/>
       <c r="AA14" s="56"/>
     </row>
-    <row r="15" spans="1:27" ht="25.5" customHeight="1">
-      <c r="A15" s="69" t="s">
+    <row r="15" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="70"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="81"/>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
       <c r="J15" s="56"/>
@@ -3547,7 +3706,7 @@
       <c r="Z15" s="56"/>
       <c r="AA15" s="56"/>
     </row>
-    <row r="16" spans="1:27" ht="51">
+    <row r="16" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
         <v>141</v>
       </c>
@@ -3590,7 +3749,7 @@
       <c r="Z16" s="56"/>
       <c r="AA16" s="56"/>
     </row>
-    <row r="17" spans="1:27" ht="51">
+    <row r="17" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
         <v>136</v>
       </c>
@@ -3633,7 +3792,7 @@
       <c r="Z17" s="56"/>
       <c r="AA17" s="56"/>
     </row>
-    <row r="18" spans="1:27" ht="51">
+    <row r="18" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
         <v>131</v>
       </c>
@@ -3676,7 +3835,7 @@
       <c r="Z18" s="56"/>
       <c r="AA18" s="56"/>
     </row>
-    <row r="19" spans="1:27" ht="63.75">
+    <row r="19" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
         <v>126</v>
       </c>
@@ -3719,7 +3878,7 @@
       <c r="Z19" s="56"/>
       <c r="AA19" s="56"/>
     </row>
-    <row r="20" spans="1:27" ht="51">
+    <row r="20" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
         <v>121</v>
       </c>
@@ -3762,7 +3921,7 @@
       <c r="Z20" s="56"/>
       <c r="AA20" s="56"/>
     </row>
-    <row r="21" spans="1:27" ht="51">
+    <row r="21" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>116</v>
       </c>
@@ -3805,7 +3964,7 @@
       <c r="Z21" s="57"/>
       <c r="AA21" s="57"/>
     </row>
-    <row r="22" spans="1:27" ht="51">
+    <row r="22" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
         <v>111</v>
       </c>
@@ -3848,7 +4007,7 @@
       <c r="Z22" s="57"/>
       <c r="AA22" s="57"/>
     </row>
-    <row r="23" spans="1:27" ht="26.25" customHeight="1">
+    <row r="23" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -3877,7 +4036,7 @@
       <c r="Z23" s="56"/>
       <c r="AA23" s="56"/>
     </row>
-    <row r="24" spans="1:27" ht="61.5" customHeight="1">
+    <row r="24" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55"/>
       <c r="B24" s="55"/>
       <c r="C24" s="50"/>
@@ -3885,7 +4044,7 @@
       <c r="E24" s="50"/>
       <c r="F24" s="50"/>
     </row>
-    <row r="25" spans="1:27" ht="12.75">
+    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="54" t="s">
         <v>16</v>
       </c>
@@ -3895,7 +4054,7 @@
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
     </row>
-    <row r="26" spans="1:27" ht="25.5">
+    <row r="26" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="53" t="s">
         <v>10</v>
       </c>
@@ -3907,7 +4066,7 @@
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
     </row>
-    <row r="27" spans="1:27" ht="12.75">
+    <row r="27" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="53" t="s">
         <v>17</v>
       </c>
@@ -3919,7 +4078,7 @@
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
     </row>
-    <row r="28" spans="1:27" ht="12.75">
+    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="53" t="s">
         <v>11</v>
       </c>
@@ -3931,7 +4090,7 @@
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
     </row>
-    <row r="29" spans="1:27" ht="12.75">
+    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
         <v>12</v>
       </c>
@@ -3943,7 +4102,7 @@
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
     </row>
-    <row r="30" spans="1:27" ht="12.75">
+    <row r="30" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="53" t="s">
         <v>13</v>
       </c>
@@ -3955,7 +4114,7 @@
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
     </row>
-    <row r="31" spans="1:27" ht="12.75">
+    <row r="31" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
         <v>18</v>
       </c>
@@ -3967,7 +4126,7 @@
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
     </row>
-    <row r="32" spans="1:27" ht="12.75">
+    <row r="32" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="53" t="s">
         <v>19</v>
       </c>
@@ -3979,7 +4138,7 @@
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="51"/>
       <c r="B33" s="51"/>
       <c r="C33" s="51"/>
@@ -3987,7 +4146,7 @@
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="50"/>
       <c r="B34" s="50"/>
       <c r="C34" s="50"/>
@@ -3995,7 +4154,7 @@
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="50"/>
       <c r="B35" s="50"/>
       <c r="C35" s="50"/>
@@ -4003,7 +4162,7 @@
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="50"/>
       <c r="B36" s="50"/>
       <c r="C36" s="50"/>
@@ -4011,7 +4170,7 @@
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="50"/>
       <c r="B37" s="50"/>
       <c r="C37" s="50"/>
@@ -4019,7 +4178,7 @@
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="50"/>
       <c r="B38" s="50"/>
       <c r="C38" s="50"/>
@@ -4027,7 +4186,7 @@
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="50"/>
       <c r="B39" s="50"/>
       <c r="C39" s="50"/>
@@ -4035,7 +4194,7 @@
       <c r="E39" s="50"/>
       <c r="F39" s="50"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="50"/>
       <c r="B40" s="50"/>
       <c r="C40" s="50"/>
@@ -4043,7 +4202,7 @@
       <c r="E40" s="50"/>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="50"/>
       <c r="B41" s="50"/>
       <c r="C41" s="50"/>
@@ -4051,7 +4210,7 @@
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="50"/>
       <c r="B42" s="50"/>
       <c r="C42" s="50"/>
@@ -4069,14 +4228,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="E7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -4087,7 +4246,7 @@
     <col min="7" max="7" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75">
+    <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4099,7 +4258,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75">
+    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -4111,7 +4270,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -4121,7 +4280,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -4133,7 +4292,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -4145,7 +4304,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75">
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -4157,7 +4316,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="12.75">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>64</v>
       </c>
@@ -4169,7 +4328,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -4179,7 +4338,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="12.75">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4187,7 +4346,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="12.75">
+    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -4216,7 +4375,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="28.5">
+    <row r="11" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -4259,7 +4418,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="35.25" customHeight="1">
+    <row r="12" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>158</v>
       </c>
@@ -4302,7 +4461,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="35.25" customHeight="1">
+    <row r="13" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>163</v>
       </c>
@@ -4345,7 +4504,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="12.75">
+    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>168</v>
       </c>
@@ -4376,14 +4535,14 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="63.75">
+    <row r="15" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>169</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="69" t="s">
         <v>164</v>
       </c>
       <c r="D15" s="27" t="s">
@@ -4392,10 +4551,10 @@
       <c r="E15" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="70" t="s">
         <v>172</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="71" t="s">
         <v>188</v>
       </c>
       <c r="H15" s="1"/>
@@ -4419,7 +4578,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="77.25" customHeight="1">
+    <row r="16" spans="1:27" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>189</v>
       </c>
@@ -4435,10 +4594,10 @@
       <c r="E16" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="F16" s="74" t="s">
+      <c r="F16" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="G16" s="73" t="s">
+      <c r="G16" s="71" t="s">
         <v>193</v>
       </c>
       <c r="H16" s="1"/>
@@ -4462,7 +4621,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="93.75" customHeight="1">
+    <row r="17" spans="1:27" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>194</v>
       </c>
@@ -4478,10 +4637,10 @@
       <c r="E17" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F17" s="74" t="s">
+      <c r="F17" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="G17" s="73" t="s">
+      <c r="G17" s="71" t="s">
         <v>198</v>
       </c>
       <c r="H17" s="1"/>
@@ -4505,7 +4664,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="82.5" customHeight="1">
+    <row r="18" spans="1:27" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>199</v>
       </c>
@@ -4521,10 +4680,10 @@
       <c r="E18" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F18" s="74" t="s">
+      <c r="F18" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="G18" s="73" t="s">
+      <c r="G18" s="71" t="s">
         <v>203</v>
       </c>
       <c r="H18" s="1"/>
@@ -4548,7 +4707,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="92.25" customHeight="1">
+    <row r="19" spans="1:27" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>204</v>
       </c>
@@ -4564,10 +4723,10 @@
       <c r="E19" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="72" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="G19" s="71" t="s">
         <v>208</v>
       </c>
       <c r="H19" s="1"/>
@@ -4591,26 +4750,26 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="84.75" customHeight="1">
-      <c r="A20" s="75" t="s">
+    <row r="20" spans="1:27" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="73" t="s">
         <v>210</v>
       </c>
       <c r="C20" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="75" t="s">
+      <c r="D20" s="73" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="F20" s="74" t="s">
+      <c r="F20" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="G20" s="71" t="s">
         <v>213</v>
       </c>
       <c r="H20" s="1"/>
@@ -4634,14 +4793,14 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="86.25" customHeight="1">
+    <row r="21" spans="1:27" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="74" t="s">
         <v>215</v>
       </c>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="75" t="s">
         <v>171</v>
       </c>
       <c r="D21" s="27" t="s">
@@ -4650,8 +4809,8 @@
       <c r="E21" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="73" t="s">
+      <c r="F21" s="76"/>
+      <c r="G21" s="71" t="s">
         <v>217</v>
       </c>
       <c r="H21" s="1"/>
@@ -4675,24 +4834,24 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" ht="51">
+    <row r="22" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="74" t="s">
         <v>219</v>
       </c>
       <c r="C22" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D22" s="75" t="s">
+      <c r="D22" s="73" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="73" t="s">
+      <c r="F22" s="76"/>
+      <c r="G22" s="71" t="s">
         <v>221</v>
       </c>
       <c r="H22" s="1"/>
@@ -4716,9 +4875,9 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="61.5" customHeight="1">
+    <row r="23" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="77" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="3"/>
@@ -4726,7 +4885,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:27" ht="12.75">
+    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>16</v>
       </c>
@@ -4736,7 +4895,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:27" ht="12.75">
+    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>10</v>
       </c>
@@ -4748,7 +4907,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:27" ht="12.75">
+    <row r="26" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>17</v>
       </c>
@@ -4760,7 +4919,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:27" ht="12.75">
+    <row r="27" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>11</v>
       </c>
@@ -4772,7 +4931,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:27" ht="12.75">
+    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>12</v>
       </c>
@@ -4784,7 +4943,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="12.75">
+    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>13</v>
       </c>
@@ -4796,7 +4955,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:27" ht="12.75">
+    <row r="30" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>18</v>
       </c>
@@ -4808,7 +4967,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:27" ht="12.75">
+    <row r="31" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>19</v>
       </c>
@@ -4820,7 +4979,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" customHeight="1">
+    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -4828,7 +4987,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4836,7 +4995,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4844,7 +5003,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4852,7 +5011,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4860,7 +5019,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4868,7 +5027,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4876,7 +5035,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4884,7 +5043,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4892,7 +5051,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -4904,4 +5063,496 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="47"/>
+    </row>
+    <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="G14" s="47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="47"/>
+    </row>
+    <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="G16" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D19" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="F19" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D20" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D21" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="47"/>
+    </row>
+    <row r="23" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D23" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="F23" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>